<commit_message>
pushing back v2.0 from svn
</commit_message>
<xml_diff>
--- a/eagle/Mecanumbot Power Board/Mecanumbot Power Board BOM.xlsx
+++ b/eagle/Mecanumbot Power Board/Mecanumbot Power Board BOM.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="375" windowWidth="22755" windowHeight="11985"/>
+    <workbookView xWindow="600" yWindow="375" windowWidth="22755" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="v1 BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="v2 BOM" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="280">
   <si>
     <t>Part</t>
   </si>
@@ -752,6 +753,108 @@
   </si>
   <si>
     <t>footprint is wrong, but should work</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MB2181SS1W01-CA/360-2178-ND/1014874</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/0297015.WXNV/F992-ND/146594</t>
+  </si>
+  <si>
+    <t>fuse</t>
+  </si>
+  <si>
+    <t>fuse holder</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/01530008Z/F065-ND/183334</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3</t>
+  </si>
+  <si>
+    <t>.1uF</t>
+  </si>
+  <si>
+    <t>C7, C8, C10</t>
+  </si>
+  <si>
+    <t>R7, R27, R28, R29, R33</t>
+  </si>
+  <si>
+    <t>R1, R2, R4, R18, R19, R20, R21, R30</t>
+  </si>
+  <si>
+    <t>BZT52C33-FDICT-ND</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
+  </si>
+  <si>
+    <t>U$2, U$3, U$4</t>
+  </si>
+  <si>
+    <t>33V Zener Diode, 500mW</t>
+  </si>
+  <si>
+    <t>CLA230TR-NDSMD</t>
+  </si>
+  <si>
+    <t>4-SOP</t>
+  </si>
+  <si>
+    <t>Digi-Key part: CLA230TR-ND</t>
+  </si>
+  <si>
+    <t>U$5, U$8, U$11</t>
+  </si>
+  <si>
+    <t>U$6, U$7, U$10</t>
+  </si>
+  <si>
+    <t>LED4, LED5, LED6</t>
+  </si>
+  <si>
+    <t>JP1, PC-CTRL</t>
+  </si>
+  <si>
+    <t>U$12, U$13, U$14, U$16, U$17, U$18</t>
+  </si>
+  <si>
+    <t>LED2, LED3</t>
+  </si>
+  <si>
+    <t>Sub-total</t>
+  </si>
+  <si>
+    <t>R3, R6, R12, R13, R14, R15, R16, R17, R23, R24, R25, R34, R37</t>
+  </si>
+  <si>
+    <t>CLA230TR-ND</t>
+  </si>
+  <si>
+    <t>JP2, JP3, JP7</t>
+  </si>
+  <si>
+    <t>USB, PWR-CTRL, I2C</t>
+  </si>
+  <si>
+    <t>311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-3.30KHRCT-ND</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>475-2816-1-ND</t>
   </si>
 </sst>
 </file>
@@ -761,7 +864,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,6 +897,18 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -844,7 +959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -863,12 +978,87 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -914,13 +1104,34 @@
   <autoFilter ref="A1:G103"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Part" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Value" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="Value" dataDxfId="11" totalsRowDxfId="10"/>
     <tableColumn id="3" name="Device"/>
-    <tableColumn id="4" name="Package" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="4" name="Package" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="5" name="Description"/>
     <tableColumn id="6" name="Digi-Key PN"/>
-    <tableColumn id="7" name="Cost" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Currency">
-      <totalsRowFormula>E5=SUBTOTAL(103,Table1[Cost])</totalsRowFormula>
+    <tableColumn id="7" name="Cost" totalsRowFunction="sum" totalsRowDxfId="7" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I30" totalsRowCount="1">
+  <autoFilter ref="A1:I29"/>
+  <sortState ref="A2:F32">
+    <sortCondition descending="1" ref="A1:A32"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Qty" totalsRowLabel="Total"/>
+    <tableColumn id="5" name="Parts"/>
+    <tableColumn id="9" name="Digi-Key PN" dataDxfId="0"/>
+    <tableColumn id="2" name="Value" dataDxfId="1" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Device"/>
+    <tableColumn id="4" name="Package" dataDxfId="6" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="Description"/>
+    <tableColumn id="10" name="Cost" totalsRowDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="11" name="Sub-total" totalsRowFunction="sum" totalsRowDxfId="2" dataCellStyle="Currency">
+      <calculatedColumnFormula>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1214,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3519,9 +3730,30 @@
       <c r="A104" t="s">
         <v>197</v>
       </c>
-      <c r="G104" s="6" t="b">
-        <f>E5=SUBTOTAL(103,Table1[Cost])</f>
-        <v>0</v>
+      <c r="G104" s="14">
+        <f>SUBTOTAL(109,Table1[Cost])</f>
+        <v>101.09870000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -3535,4 +3767,891 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="1">
+        <v>330</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="I3" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.8399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="I4" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="I6" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I7" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" t="s">
+        <v>261</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="I8" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="I9" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="I10" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="I11" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.52499999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="I12" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I13" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="I14" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1206</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="I16" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="I17" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3.05</v>
+      </c>
+      <c r="I19" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="I20" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E21" t="s">
+        <v>262</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G21" t="s">
+        <v>264</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="I21" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" t="s">
+        <v>183</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="I22" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I23" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>274</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="I24" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="I25" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I26" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27" t="s">
+        <v>190</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="I27" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H28" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="I28" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="I29" s="2">
+        <f>Table2[[#This Row],[Cost]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6">
+        <f>SUBTOTAL(109,Table2[Sub-total])</f>
+        <v>41.083400000000012</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>